<commit_message>
leer a partir de la 4ta fila
</commit_message>
<xml_diff>
--- a/static/productos.xlsx
+++ b/static/productos.xlsx
@@ -26,7 +26,7 @@
     <author>Miguel Angel Soto González</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Categoria</t>
   </si>
@@ -84,7 +84,13 @@
     <t>Cuál es tu talla</t>
   </si>
   <si>
-    <t>Tallas Disponible</t>
+    <t>Talla 1</t>
+  </si>
+  <si>
+    <t>Talla 2</t>
+  </si>
+  <si>
+    <t>Talla 3</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -171,11 +177,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -226,14 +241,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -549,93 +562,105 @@
     <col min="11" max="11" width="24.7109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1" ht="42.95" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+    </row>
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="42.95" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -647,13 +672,15 @@
       <c r="I5" s="5"/>
       <c r="J5" s="3"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="14"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
@@ -663,12 +690,14 @@
       <c r="J6" s="3"/>
       <c r="K6" s="12"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
@@ -676,11 +705,13 @@
       <c r="H7" s="4"/>
       <c r="I7" s="5"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="12"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -694,11 +725,13 @@
       <c r="K8" s="12"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
@@ -709,8 +742,10 @@
       <c r="K9" s="12"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13" ht="125.25" customHeight="1">
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -724,11 +759,13 @@
       <c r="K10" s="12"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
@@ -739,8 +776,10 @@
       <c r="K11" s="12"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -754,11 +793,13 @@
       <c r="K12" s="12"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" ht="125.25" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
@@ -769,11 +810,13 @@
       <c r="K13" s="12"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
@@ -784,8 +827,10 @@
       <c r="K14" s="12"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -799,11 +844,13 @@
       <c r="K15" s="12"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
@@ -814,8 +861,10 @@
       <c r="K16" s="12"/>
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -829,8 +878,10 @@
       <c r="K17" s="12"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -844,8 +895,10 @@
       <c r="K18" s="12"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -859,13 +912,15 @@
       <c r="K19" s="12"/>
       <c r="L19" s="14"/>
       <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -874,13 +929,15 @@
       <c r="K20" s="12"/>
       <c r="L20" s="14"/>
       <c r="M20" s="14"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -889,8 +946,10 @@
       <c r="K21" s="12"/>
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -904,13 +963,15 @@
       <c r="K22" s="12"/>
       <c r="L22" s="14"/>
       <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -919,13 +980,15 @@
       <c r="K23" s="12"/>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -934,11 +997,13 @@
       <c r="K24" s="12"/>
       <c r="L24" s="14"/>
       <c r="M24" s="14"/>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
@@ -949,11 +1014,13 @@
       <c r="K25" s="12"/>
       <c r="L25" s="14"/>
       <c r="M25" s="14"/>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="7"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
@@ -964,11 +1031,13 @@
       <c r="K26" s="12"/>
       <c r="L26" s="14"/>
       <c r="M26" s="14"/>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="7"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
@@ -979,11 +1048,13 @@
       <c r="K27" s="12"/>
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="2"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
@@ -994,11 +1065,13 @@
       <c r="K28" s="12"/>
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
@@ -1009,11 +1082,13 @@
       <c r="K29" s="12"/>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="2"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
@@ -1024,8 +1099,10 @@
       <c r="K30" s="12"/>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1039,8 +1116,10 @@
       <c r="K31" s="12"/>
       <c r="L31" s="14"/>
       <c r="M31" s="14"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1054,8 +1133,10 @@
       <c r="K32" s="12"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1069,11 +1150,13 @@
       <c r="K33" s="12"/>
       <c r="L33" s="14"/>
       <c r="M33" s="14"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="7"/>
+      <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
@@ -1084,11 +1167,13 @@
       <c r="K34" s="12"/>
       <c r="L34" s="14"/>
       <c r="M34" s="14"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="7"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
@@ -1099,11 +1184,13 @@
       <c r="K35" s="12"/>
       <c r="L35" s="14"/>
       <c r="M35" s="14"/>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="7"/>
+      <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="3"/>
       <c r="F36" s="4"/>
@@ -1114,13 +1201,15 @@
       <c r="K36" s="12"/>
       <c r="L36" s="14"/>
       <c r="M36" s="14"/>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="7"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="9"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -1129,8 +1218,64 @@
       <c r="K37" s="12"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>